<commit_message>
adding get to the webapp
</commit_message>
<xml_diff>
--- a/web_app/apps/tmp_data_return.xlsx
+++ b/web_app/apps/tmp_data_return.xlsx
@@ -1,40 +1,78 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Commodity_-_USD_Unhedged_%y/y</t>
+  </si>
+  <si>
+    <t>Global_Property_USD_Unhedged_%y/y</t>
+  </si>
+  <si>
+    <t>Hedge_Fund_DJ_-_USD_Unhedged_%y/y</t>
+  </si>
+  <si>
+    <t>Infrastructure_Debt_-_USD_Unhedged_%y/y</t>
+  </si>
+  <si>
+    <t>Infrastructure_Equity_Listed_-_USD_Unhedged_%y/y</t>
+  </si>
+  <si>
+    <t>Infrastructure_Equity_USD_Unhedged_%y/y</t>
+  </si>
+  <si>
+    <t>Nature_Capital_-_USD_Hedged_%y/y</t>
+  </si>
+  <si>
+    <t>Private_Equity_USD_Unhedged_%y/y</t>
+  </si>
+  <si>
+    <t>UK_Property_Direct_-_USD_Unhedged_%y/y</t>
+  </si>
+  <si>
+    <t>QUARTER</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,96 +87,38 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -426,3276 +406,2932 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>QUARTER</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Commodity_-_USD_Unhedged_%y/y</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Global_Property_USD_Unhedged_%y/y</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Hedge_Fund_DJ_-_USD_Unhedged_%y/y</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Infrastructure_Debt_-_USD_Unhedged_%y/y</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Infrastructure_Equity_Listed_-_USD_Unhedged_%y/y</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Infrastructure_Equity_USD_Unhedged_%y/y</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Nature_Capital_-_USD_Hedged_%y/y</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Private_Equity_USD_Unhedged_%y/y</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>UK_Property_Direct_-_USD_Unhedged_%y/y</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2">
         <v>34243</v>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2">
         <v>34335</v>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
+      <c r="I3">
         <v>0.1015058876811594</v>
       </c>
-      <c r="J3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2">
         <v>34425</v>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="n">
+      <c r="I4">
         <v>0.02983502081513079</v>
       </c>
-      <c r="J4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2">
         <v>34516</v>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="n">
+      <c r="I5">
         <v>0.03668122270742358</v>
       </c>
-      <c r="J5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="2">
         <v>34608</v>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="n">
+      <c r="I6">
         <v>0.001612709110603072</v>
       </c>
-      <c r="J6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2">
         <v>34700</v>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="n">
+      <c r="I7">
         <v>0.05486398154378547</v>
       </c>
-      <c r="J7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="2">
         <v>34790</v>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="n">
+      <c r="I8">
         <v>0.06624900330333738</v>
       </c>
-      <c r="J8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="2">
         <v>34881</v>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="n">
+      <c r="I9">
         <v>0.1348417836463476</v>
       </c>
-      <c r="J9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="2">
         <v>34973</v>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="n">
+      <c r="I10">
         <v>0.04460217645065345</v>
       </c>
-      <c r="J10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2">
         <v>35065</v>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="n">
+      <c r="I11">
         <v>0.08332281960240051</v>
       </c>
-      <c r="J11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="n">
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="2">
         <v>35156</v>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="n">
+      <c r="I12">
         <v>0.1113200013309821</v>
       </c>
-      <c r="J12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="n">
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="2">
         <v>35247</v>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="n">
+      <c r="I13">
         <v>0.03702262077638219</v>
       </c>
-      <c r="J13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="n">
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="2">
         <v>35339</v>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="n">
+      <c r="I14">
         <v>0.01133246715749947</v>
       </c>
-      <c r="J14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="n">
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="2">
         <v>35431</v>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="n">
+      <c r="I15">
         <v>-0.04148169295553483</v>
       </c>
-      <c r="J15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="n">
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="2">
         <v>35521</v>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="n">
+      <c r="I16">
         <v>0.0865091066136503</v>
       </c>
-      <c r="J16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="n">
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="2">
         <v>35612</v>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="n">
+      <c r="I17">
         <v>-0.08278735710956997</v>
       </c>
-      <c r="J17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="n">
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="2">
         <v>35704</v>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="n">
+      <c r="I18">
         <v>0.02695836695657383</v>
       </c>
-      <c r="J18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="n">
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="2">
         <v>35796</v>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="n">
+      <c r="I19">
         <v>0.17678472687058</v>
       </c>
-      <c r="J19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="n">
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="2">
         <v>35886</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>-0.08182959833990344</v>
       </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="n">
+      <c r="D20">
         <v>0.02825154337135083</v>
       </c>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="n">
+      <c r="I20">
         <v>0.04752012464294975</v>
       </c>
-      <c r="J20" t="n">
+      <c r="J20">
         <v>-0.06648911596796503</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="2" t="n">
+    <row r="21" spans="1:10">
+      <c r="A21" s="2">
         <v>35977</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>-0.05148403329383722</v>
       </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="n">
+      <c r="D21">
         <v>-0.08873511753332652</v>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="n">
+      <c r="I21">
         <v>-0.2024694855631891</v>
       </c>
-      <c r="J21" t="n">
+      <c r="J21">
         <v>-0.0632882603695869</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="2" t="n">
+    <row r="22" spans="1:10">
+      <c r="A22" s="2">
         <v>36069</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>-0.1302175304396104</v>
       </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="n">
+      <c r="D22">
         <v>-0.00346175321049691</v>
       </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="n">
+      <c r="I22">
         <v>0.1136289630265535</v>
       </c>
-      <c r="J22" t="n">
+      <c r="J22">
         <v>-0.06515259874725643</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="2" t="n">
+    <row r="23" spans="1:10">
+      <c r="A23" s="2">
         <v>36161</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>0.05304266108727251</v>
       </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="n">
+      <c r="D23">
         <v>0.007003585835948067</v>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="n">
+      <c r="I23">
         <v>0.1735137362272228</v>
       </c>
-      <c r="J23" t="n">
+      <c r="J23">
         <v>0.06235456620848678</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="2" t="n">
+    <row r="24" spans="1:10">
+      <c r="A24" s="2">
         <v>36251</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>0.03106609754249479</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24">
         <v>0.09780911939043957</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24">
         <v>0.06125855449841433</v>
       </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="n">
+      <c r="I24">
         <v>0.1272226878383582</v>
       </c>
-      <c r="J24" t="n">
+      <c r="J24">
         <v>0.03195967541798606</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="2" t="n">
+    <row r="25" spans="1:10">
+      <c r="A25" s="2">
         <v>36342</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>0.1326294817464011</v>
       </c>
-      <c r="C25" t="n">
+      <c r="C25">
         <v>-0.06388775642109246</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25">
         <v>-0.009646639404424895</v>
       </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="n">
+      <c r="I25">
         <v>0.07611000030142567</v>
       </c>
-      <c r="J25" t="n">
+      <c r="J25">
         <v>0.0294927898809636</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="2" t="n">
+    <row r="26" spans="1:10">
+      <c r="A26" s="2">
         <v>36434</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>0.01113818559317159</v>
       </c>
-      <c r="C26" t="n">
+      <c r="C26">
         <v>0.06222514924263356</v>
       </c>
-      <c r="D26" t="n">
+      <c r="D26">
         <v>0.1661725780836421</v>
       </c>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="n">
+      <c r="I26">
         <v>0.6373550447237215</v>
       </c>
-      <c r="J26" t="n">
+      <c r="J26">
         <v>-0.0375052214974142</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="2" t="n">
+    <row r="27" spans="1:10">
+      <c r="A27" s="2">
         <v>36526</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>0.08304041866003109</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27">
         <v>-0.02479999999999993</v>
       </c>
-      <c r="D27" t="n">
+      <c r="D27">
         <v>0.0413091833492214</v>
       </c>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="n">
+      <c r="I27">
         <v>0.09026368011678554</v>
       </c>
-      <c r="J27" t="n">
+      <c r="J27">
         <v>-0.03225475229205244</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="2" t="n">
+    <row r="28" spans="1:10">
+      <c r="A28" s="2">
         <v>36617</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>0.0790762586896987</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28">
         <v>0.03609515996718615</v>
       </c>
-      <c r="D28" t="n">
+      <c r="D28">
         <v>-0.02288678669514799</v>
       </c>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="n">
+      <c r="H28">
         <v>0.13011483705313</v>
       </c>
-      <c r="I28" t="n">
+      <c r="I28">
         <v>-0.1941022945400721</v>
       </c>
-      <c r="J28" t="n">
+      <c r="J28">
         <v>0.01490103168422952</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="2" t="n">
+    <row r="29" spans="1:10">
+      <c r="A29" s="2">
         <v>36708</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>0.0368481417311306</v>
       </c>
-      <c r="C29" t="n">
+      <c r="C29">
         <v>0.07487133808392721</v>
       </c>
-      <c r="D29" t="n">
+      <c r="D29">
         <v>0.03082894619434295</v>
       </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="n">
+      <c r="H29">
         <v>0.1682741036252844</v>
       </c>
-      <c r="I29" t="n">
+      <c r="I29">
         <v>-0.03818096857517417</v>
       </c>
-      <c r="J29" t="n">
+      <c r="J29">
         <v>0.04594597919544463</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="2" t="n">
+    <row r="30" spans="1:10">
+      <c r="A30" s="2">
         <v>36800</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>0.08802866624302763</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30">
         <v>0.04821140831453441</v>
       </c>
-      <c r="D30" t="n">
+      <c r="D30">
         <v>-0.0003462454014283578</v>
       </c>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="n">
+      <c r="H30">
         <v>-0.006796237623370671</v>
       </c>
-      <c r="I30" t="n">
+      <c r="I30">
         <v>-0.225642548195332</v>
       </c>
-      <c r="J30" t="n">
+      <c r="J30">
         <v>0.0497567423231895</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" s="2" t="n">
+    <row r="31" spans="1:10">
+      <c r="A31" s="2">
         <v>36892</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>-0.06903637848331945</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31">
         <v>-0.05046512240756851</v>
       </c>
-      <c r="D31" t="n">
+      <c r="D31">
         <v>0.0001298869983115125</v>
       </c>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="n">
+      <c r="H31">
         <v>0.05023629757822645</v>
       </c>
-      <c r="I31" t="n">
+      <c r="I31">
         <v>-0.1202171507245618</v>
       </c>
-      <c r="J31" t="n">
+      <c r="J31">
         <v>-0.0354158390653696</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" s="2" t="n">
+    <row r="32" spans="1:10">
+      <c r="A32" s="2">
         <v>36982</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>-0.02694146417970278</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32">
         <v>0.06015023682652454</v>
       </c>
-      <c r="D32" t="n">
+      <c r="D32">
         <v>0.0211255411255411</v>
       </c>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="n">
+      <c r="H32">
         <v>0.01163641203785803</v>
       </c>
-      <c r="I32" t="n">
+      <c r="I32">
         <v>-0.01618414666759116</v>
       </c>
-      <c r="J32" t="n">
+      <c r="J32">
         <v>0.01771131165279405</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="2" t="n">
+    <row r="33" spans="1:10">
+      <c r="A33" s="2">
         <v>37073</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>-0.05572701820157244</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33">
         <v>-0.09830014485418603</v>
       </c>
-      <c r="D33" t="n">
+      <c r="D33">
         <v>0.0005511276920466823</v>
       </c>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="n">
+      <c r="H33">
         <v>-0.07165647389733953</v>
       </c>
-      <c r="I33" t="n">
+      <c r="I33">
         <v>-0.2370908798034813</v>
       </c>
-      <c r="J33" t="n">
+      <c r="J33">
         <v>-0.01286943217744851</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" s="2" t="n">
+    <row r="34" spans="1:10">
+      <c r="A34" s="2">
         <v>37165</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>-0.05901579233521737</v>
       </c>
-      <c r="C34" t="n">
+      <c r="C34">
         <v>0.05973890238355617</v>
       </c>
-      <c r="D34" t="n">
+      <c r="D34">
         <v>0.02186348036100161</v>
       </c>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="n">
+      <c r="H34">
         <v>0.113633703473734</v>
       </c>
-      <c r="I34" t="n">
+      <c r="I34">
         <v>0.13726758072817</v>
       </c>
-      <c r="J34" t="n">
+      <c r="J34">
         <v>-0.002177441530583857</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" s="2" t="n">
+    <row r="35" spans="1:10">
+      <c r="A35" s="2">
         <v>37257</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>0.1232103625968302</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35">
         <v>0.05375961134549723</v>
       </c>
-      <c r="D35" t="n">
+      <c r="D35">
         <v>0.007131898660695857</v>
       </c>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="n">
+      <c r="H35">
         <v>0.002061776534596715</v>
       </c>
-      <c r="I35" t="n">
+      <c r="I35">
         <v>0.02614265325303733</v>
       </c>
-      <c r="J35" t="n">
+      <c r="J35">
         <v>0.06634649910921664</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="2" t="n">
+    <row r="36" spans="1:10">
+      <c r="A36" s="2">
         <v>37347</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>0.003726477730856326</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36">
         <v>0.05438804780185968</v>
       </c>
-      <c r="D36" t="n">
+      <c r="D36">
         <v>0.006175635061138829</v>
       </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="n">
+      <c r="H36">
         <v>0.06085139748025958</v>
       </c>
-      <c r="I36" t="n">
+      <c r="I36">
         <v>-0.02819051496030944</v>
       </c>
-      <c r="J36" t="n">
+      <c r="J36">
         <v>0.08718970257196057</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" s="2" t="n">
+    <row r="37" spans="1:10">
+      <c r="A37" s="2">
         <v>37438</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>0.07270343553529379</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37">
         <v>-0.1007323147227313</v>
       </c>
-      <c r="D37" t="n">
+      <c r="D37">
         <v>-0.004337329677973623</v>
       </c>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="n">
+      <c r="H37">
         <v>-0.008975931569804696</v>
       </c>
-      <c r="I37" t="n">
+      <c r="I37">
         <v>-0.2464248728779046</v>
       </c>
-      <c r="J37" t="n">
+      <c r="J37">
         <v>-0.07406396764715228</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" s="2" t="n">
+    <row r="38" spans="1:10">
+      <c r="A38" s="2">
         <v>37530</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38">
         <v>0.04108774756256772</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38">
         <v>0.02903676893970553</v>
       </c>
-      <c r="D38" t="n">
+      <c r="D38">
         <v>0.02128796284880607</v>
       </c>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="n">
+      <c r="H38">
         <v>-0.007075487176147366</v>
       </c>
-      <c r="I38" t="n">
+      <c r="I38">
         <v>0.09474545651066202</v>
       </c>
-      <c r="J38" t="n">
+      <c r="J38">
         <v>0.06820470378430721</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" s="2" t="n">
+    <row r="39" spans="1:10">
+      <c r="A39" s="2">
         <v>37622</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39">
         <v>0.02922076189561418</v>
       </c>
-      <c r="C39" t="n">
+      <c r="C39">
         <v>-0.01731059596767026</v>
       </c>
-      <c r="D39" t="n">
+      <c r="D39">
         <v>0.02225262564886732</v>
       </c>
-      <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="n">
+      <c r="H39">
         <v>-0.017170971597401</v>
       </c>
-      <c r="I39" t="n">
+      <c r="I39">
         <v>-0.1004668613097505</v>
       </c>
-      <c r="J39" t="n">
+      <c r="J39">
         <v>-0.07831175811567492</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" s="2" t="n">
+    <row r="40" spans="1:10">
+      <c r="A40" s="2">
         <v>37712</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40">
         <v>0.02586104097429964</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40">
         <v>0.144367820247467</v>
       </c>
-      <c r="D40" t="n">
+      <c r="D40">
         <v>0.05593607305936077</v>
       </c>
-      <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="n">
+      <c r="H40">
         <v>0.08483602116932065</v>
       </c>
-      <c r="I40" t="n">
+      <c r="I40">
         <v>0.2795565730055192</v>
       </c>
-      <c r="J40" t="n">
+      <c r="J40">
         <v>0.175456249479863</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" s="2" t="n">
+    <row r="41" spans="1:10">
+      <c r="A41" s="2">
         <v>37803</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41">
         <v>0.04661764334268304</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41">
         <v>0.1185413935267821</v>
       </c>
-      <c r="D41" t="n">
+      <c r="D41">
         <v>0.02370922646784712</v>
       </c>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="n">
+      <c r="H41">
         <v>0.002435900695378912</v>
       </c>
-      <c r="I41" t="n">
+      <c r="I41">
         <v>0.139893388885485</v>
       </c>
-      <c r="J41" t="n">
+      <c r="J41">
         <v>0.05477277433832195</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="2" t="n">
+    <row r="42" spans="1:10">
+      <c r="A42" s="2">
         <v>37895</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42">
         <v>0.1214936573164196</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C42">
         <v>0.1185188846444434</v>
       </c>
-      <c r="D42" t="n">
+      <c r="D42">
         <v>0.04471796365755054</v>
       </c>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="n">
+      <c r="H42">
         <v>0.1006024033152468</v>
       </c>
-      <c r="I42" t="n">
+      <c r="I42">
         <v>0.1454510271874092</v>
       </c>
-      <c r="J42" t="n">
+      <c r="J42">
         <v>0.1722650222508924</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" s="2" t="n">
+    <row r="43" spans="1:10">
+      <c r="A43" s="2">
         <v>37987</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43">
         <v>0.1176668144965103</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C43">
         <v>0.1348984899752539</v>
       </c>
-      <c r="D43" t="n">
+      <c r="D43">
         <v>0.03419429049461464</v>
       </c>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="n">
+      <c r="H43">
         <v>0.006069830717041702</v>
       </c>
-      <c r="I43" t="n">
+      <c r="I43">
         <v>0.1095625568976359</v>
       </c>
-      <c r="J43" t="n">
+      <c r="J43">
         <v>0.0982862724270821</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" s="2" t="n">
+    <row r="44" spans="1:10">
+      <c r="A44" s="2">
         <v>38078</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44">
         <v>-0.04249991332051761</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C44">
         <v>-0.04127335532353971</v>
       </c>
-      <c r="D44" t="n">
+      <c r="D44">
         <v>-0.004718570947084499</v>
       </c>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="n">
+      <c r="H44">
         <v>0.06344041662789346</v>
       </c>
-      <c r="I44" t="n">
+      <c r="I44">
         <v>-0.04939733558891946</v>
       </c>
-      <c r="J44" t="n">
+      <c r="J44">
         <v>0.02171216796222142</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" s="2" t="n">
+    <row r="45" spans="1:10">
+      <c r="A45" s="2">
         <v>38169</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45">
         <v>0.06752499547365653</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C45">
         <v>0.07574395005714885</v>
       </c>
-      <c r="D45" t="n">
+      <c r="D45">
         <v>0.008364375211649122</v>
       </c>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="n">
+      <c r="H45">
         <v>0.04513500787691949</v>
       </c>
-      <c r="I45" t="n">
+      <c r="I45">
         <v>-0.006184099301508095</v>
       </c>
-      <c r="J45" t="n">
+      <c r="J45">
         <v>0.04125947910462147</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="2" t="n">
+    <row r="46" spans="1:10">
+      <c r="A46" s="2">
         <v>38261</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46">
         <v>-0.04459763010311757</v>
       </c>
-      <c r="C46" t="n">
+      <c r="C46">
         <v>0.1786993290617651</v>
       </c>
-      <c r="D46" t="n">
+      <c r="D46">
         <v>0.05635221815495184</v>
       </c>
-      <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="n">
+      <c r="H46">
         <v>0.2665770616729743</v>
       </c>
-      <c r="I46" t="n">
+      <c r="I46">
         <v>0.1825409615901155</v>
       </c>
-      <c r="J46" t="n">
+      <c r="J46">
         <v>0.1851726716320319</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" s="2" t="n">
+    <row r="47" spans="1:10">
+      <c r="A47" s="2">
         <v>38353</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47">
         <v>0.1203850174559655</v>
       </c>
-      <c r="C47" t="n">
+      <c r="C47">
         <v>-0.0492072570866412</v>
       </c>
-      <c r="D47" t="n">
+      <c r="D47">
         <v>0.00934668574153541</v>
       </c>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr"/>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="n">
+      <c r="H47">
         <v>0.2704784205288557</v>
       </c>
-      <c r="I47" t="n">
+      <c r="I47">
         <v>0.01401444600917645</v>
       </c>
-      <c r="J47" t="n">
+      <c r="J47">
         <v>-0.04304858738264639</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" s="2" t="n">
+    <row r="48" spans="1:10">
+      <c r="A48" s="2">
         <v>38443</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48">
         <v>-0.04992746785347102</v>
       </c>
-      <c r="C48" t="n">
+      <c r="C48">
         <v>0.09286735229148535</v>
       </c>
-      <c r="D48" t="n">
+      <c r="D48">
         <v>0.004031623043245336</v>
       </c>
-      <c r="E48" t="n">
+      <c r="E48">
         <v>0.04361999999999999</v>
       </c>
-      <c r="F48" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="n">
+      <c r="H48">
         <v>0.3383069047191252</v>
       </c>
-      <c r="I48" t="n">
+      <c r="I48">
         <v>0.01660581352806334</v>
       </c>
-      <c r="J48" t="n">
+      <c r="J48">
         <v>-0.0008471698657698257</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" s="2" t="n">
+    <row r="49" spans="1:10">
+      <c r="A49" s="2">
         <v>38534</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49">
         <v>0.175976162945833</v>
       </c>
-      <c r="C49" t="n">
+      <c r="C49">
         <v>0.06076058620446689</v>
       </c>
-      <c r="D49" t="n">
+      <c r="D49">
         <v>0.0449540420993193</v>
       </c>
-      <c r="E49" t="n">
+      <c r="E49">
         <v>0.009840746631916142</v>
       </c>
-      <c r="F49" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="n">
+      <c r="H49">
         <v>0.150759593673417</v>
       </c>
-      <c r="I49" t="n">
+      <c r="I49">
         <v>0.1023995064376106</v>
       </c>
-      <c r="J49" t="n">
+      <c r="J49">
         <v>0.02761225642201359</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" s="2" t="n">
+    <row r="50" spans="1:10">
+      <c r="A50" s="2">
         <v>38626</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>-0.03046174791060019</v>
       </c>
-      <c r="C50" t="n">
+      <c r="C50">
         <v>0.04653653595476692</v>
       </c>
-      <c r="D50" t="n">
+      <c r="D50">
         <v>0.01615130591413982</v>
       </c>
-      <c r="E50" t="n">
+      <c r="E50">
         <v>0.008900359620074072</v>
       </c>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="n">
+      <c r="H50">
         <v>0.02605309215624585</v>
       </c>
-      <c r="I50" t="n">
+      <c r="I50">
         <v>0.06698424331256869</v>
       </c>
-      <c r="J50" t="n">
+      <c r="J50">
         <v>0.04448010978900818</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" s="2" t="n">
+    <row r="51" spans="1:10">
+      <c r="A51" s="2">
         <v>38718</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51">
         <v>-0.02403055420120259</v>
       </c>
-      <c r="C51" t="n">
+      <c r="C51">
         <v>0.1398514851485149</v>
       </c>
-      <c r="D51" t="n">
+      <c r="D51">
         <v>0.05462656582368242</v>
       </c>
-      <c r="E51" t="n">
+      <c r="E51">
         <v>-0.001119188917208302</v>
       </c>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="n">
+      <c r="H51">
         <v>0.09145480633031355</v>
       </c>
-      <c r="I51" t="n">
+      <c r="I51">
         <v>0.0861260451204815</v>
       </c>
-      <c r="J51" t="n">
+      <c r="J51">
         <v>0.1120043579486552</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="2" t="n">
+    <row r="52" spans="1:10">
+      <c r="A52" s="2">
         <v>38808</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52">
         <v>0.06126418368264508</v>
       </c>
-      <c r="C52" t="n">
+      <c r="C52">
         <v>-0.003695815585066375</v>
       </c>
-      <c r="D52" t="n">
+      <c r="D52">
         <v>0.007815782838893837</v>
       </c>
-      <c r="E52" t="n">
+      <c r="E52">
         <v>-0.004491187104549543</v>
       </c>
-      <c r="F52" t="inlineStr"/>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="n">
+      <c r="H52">
         <v>0.1428624619775849</v>
       </c>
-      <c r="I52" t="n">
+      <c r="I52">
         <v>-0.04375021558910452</v>
       </c>
-      <c r="J52" t="n">
+      <c r="J52">
         <v>0.04479012916674097</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" s="2" t="n">
+    <row r="53" spans="1:10">
+      <c r="A53" s="2">
         <v>38899</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53">
         <v>-0.06499880747649467</v>
       </c>
-      <c r="C53" t="n">
+      <c r="C53">
         <v>0.09918613992804493</v>
       </c>
-      <c r="D53" t="n">
+      <c r="D53">
         <v>0.01273070936179677</v>
       </c>
-      <c r="E53" t="n">
+      <c r="E53">
         <v>0.02793882588833929</v>
       </c>
-      <c r="F53" t="inlineStr"/>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="n">
+      <c r="H53">
         <v>0.03074329446937307</v>
       </c>
-      <c r="I53" t="n">
+      <c r="I53">
         <v>0.06798451290190721</v>
       </c>
-      <c r="J53" t="n">
+      <c r="J53">
         <v>0.08937392417924483</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" s="2" t="n">
+    <row r="54" spans="1:10">
+      <c r="A54" s="2">
         <v>38991</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B54">
         <v>0.05398066724843931</v>
       </c>
-      <c r="C54" t="n">
+      <c r="C54">
         <v>0.1404002720171853</v>
       </c>
-      <c r="D54" t="n">
+      <c r="D54">
         <v>0.05783059779327027</v>
       </c>
-      <c r="E54" t="n">
+      <c r="E54">
         <v>-0.002640658784560768</v>
       </c>
-      <c r="F54" t="inlineStr"/>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="n">
+      <c r="H54">
         <v>0.09902816588115404</v>
       </c>
-      <c r="I54" t="n">
+      <c r="I54">
         <v>0.1421470389551902</v>
       </c>
-      <c r="J54" t="n">
+      <c r="J54">
         <v>0.1785360425589302</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" s="2" t="n">
+    <row r="55" spans="1:10">
+      <c r="A55" s="2">
         <v>39083</v>
       </c>
-      <c r="B55" t="n">
+      <c r="B55">
         <v>0.04594886361826989</v>
       </c>
-      <c r="C55" t="n">
+      <c r="C55">
         <v>0.06222622245505316</v>
       </c>
-      <c r="D55" t="n">
+      <c r="D55">
         <v>0.03339301004125472</v>
       </c>
-      <c r="E55" t="n">
+      <c r="E55">
         <v>-0.001817376704367213</v>
       </c>
-      <c r="F55" t="inlineStr"/>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="n">
+      <c r="H55">
         <v>0.06934182129828148</v>
       </c>
-      <c r="I55" t="n">
+      <c r="I55">
         <v>0.07106771616286567</v>
       </c>
-      <c r="J55" t="n">
+      <c r="J55">
         <v>-0.01467969314444528</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" s="2" t="n">
+    <row r="56" spans="1:10">
+      <c r="A56" s="2">
         <v>39173</v>
       </c>
-      <c r="B56" t="n">
+      <c r="B56">
         <v>-0.001287859413247605</v>
       </c>
-      <c r="C56" t="n">
+      <c r="C56">
         <v>-0.05851274531150386</v>
       </c>
-      <c r="D56" t="n">
+      <c r="D56">
         <v>0.05189816209701714</v>
       </c>
-      <c r="E56" t="n">
+      <c r="E56">
         <v>-0.01191301374294151</v>
       </c>
-      <c r="F56" t="inlineStr"/>
-      <c r="G56" t="n">
+      <c r="G56">
         <v>0.06744637460000003</v>
       </c>
-      <c r="H56" t="n">
+      <c r="H56">
         <v>0.03736054081077289</v>
       </c>
-      <c r="I56" t="n">
+      <c r="I56">
         <v>0.03431043210160589</v>
       </c>
-      <c r="J56" t="n">
+      <c r="J56">
         <v>-0.0694425383091839</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" s="2" t="n">
+    <row r="57" spans="1:10">
+      <c r="A57" s="2">
         <v>39264</v>
       </c>
-      <c r="B57" t="n">
+      <c r="B57">
         <v>0.06242740733288832</v>
       </c>
-      <c r="C57" t="n">
+      <c r="C57">
         <v>0.03655675491927979</v>
       </c>
-      <c r="D57" t="n">
+      <c r="D57">
         <v>0.01129013008712265</v>
       </c>
-      <c r="E57" t="n">
+      <c r="E57">
         <v>0.03230694402873402</v>
       </c>
-      <c r="F57" t="inlineStr"/>
-      <c r="G57" t="n">
+      <c r="G57">
         <v>-0.02502224030692779</v>
       </c>
-      <c r="H57" t="n">
+      <c r="H57">
         <v>0.01799116218570185</v>
       </c>
-      <c r="I57" t="n">
+      <c r="I57">
         <v>-0.04652394045362718</v>
       </c>
-      <c r="J57" t="n">
+      <c r="J57">
         <v>-0.04271063810049402</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" s="2" t="n">
+    <row r="58" spans="1:10">
+      <c r="A58" s="2">
         <v>39356</v>
       </c>
-      <c r="B58" t="n">
+      <c r="B58">
         <v>0.04729603709538122</v>
       </c>
-      <c r="C58" t="n">
+      <c r="C58">
         <v>-0.1024585096259818</v>
       </c>
-      <c r="D58" t="n">
+      <c r="D58">
         <v>0.0239331570996979</v>
       </c>
-      <c r="E58" t="n">
+      <c r="E58">
         <v>0.02338582534476186</v>
       </c>
-      <c r="F58" t="inlineStr"/>
-      <c r="G58" t="n">
+      <c r="G58">
         <v>0.05441097286942043</v>
       </c>
-      <c r="H58" t="n">
+      <c r="H58">
         <v>0.08720284894055164</v>
       </c>
-      <c r="I58" t="n">
+      <c r="I58">
         <v>-0.1042606703404897</v>
       </c>
-      <c r="J58" t="n">
+      <c r="J58">
         <v>-0.117683687227966</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" s="2" t="n">
+    <row r="59" spans="1:10">
+      <c r="A59" s="2">
         <v>39448</v>
       </c>
-      <c r="B59" t="n">
+      <c r="B59">
         <v>0.09604646702649378</v>
       </c>
-      <c r="C59" t="n">
+      <c r="C59">
         <v>-0.05629264026738701</v>
       </c>
-      <c r="D59" t="n">
+      <c r="D59">
         <v>-0.02010050251256279</v>
       </c>
-      <c r="E59" t="n">
+      <c r="E59">
         <v>0.02908443783367409</v>
       </c>
-      <c r="F59" t="inlineStr"/>
-      <c r="G59" t="n">
+      <c r="G59">
         <v>0.0283642605032921</v>
       </c>
-      <c r="H59" t="n">
+      <c r="H59">
         <v>0.04950511131988033</v>
       </c>
-      <c r="I59" t="n">
+      <c r="I59">
         <v>-0.07360195869038633</v>
       </c>
-      <c r="J59" t="n">
+      <c r="J59">
         <v>0.0125335382811933</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" s="2" t="n">
+    <row r="60" spans="1:10">
+      <c r="A60" s="2">
         <v>39539</v>
       </c>
-      <c r="B60" t="n">
+      <c r="B60">
         <v>0.1607590127135381</v>
       </c>
-      <c r="C60" t="n">
+      <c r="C60">
         <v>-0.0855976794815646</v>
       </c>
-      <c r="D60" t="n">
+      <c r="D60">
         <v>0.02575864502470004</v>
       </c>
-      <c r="E60" t="n">
+      <c r="E60">
         <v>-0.04561566522128158</v>
       </c>
-      <c r="F60" t="inlineStr"/>
-      <c r="G60" t="n">
+      <c r="G60">
         <v>0.07627470783330725</v>
       </c>
-      <c r="H60" t="n">
+      <c r="H60">
         <v>0.003795395453481731</v>
       </c>
-      <c r="I60" t="n">
+      <c r="I60">
         <v>-0.08900335140241566</v>
       </c>
-      <c r="J60" t="n">
+      <c r="J60">
         <v>-0.1342363999468282</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" s="2" t="n">
+    <row r="61" spans="1:10">
+      <c r="A61" s="2">
         <v>39630</v>
       </c>
-      <c r="B61" t="n">
+      <c r="B61">
         <v>-0.2769614757611063</v>
       </c>
-      <c r="C61" t="n">
+      <c r="C61">
         <v>-0.1041057855828966</v>
       </c>
-      <c r="D61" t="n">
+      <c r="D61">
         <v>-0.1032679738562092</v>
       </c>
-      <c r="E61" t="n">
+      <c r="E61">
         <v>0.03809609663751923</v>
       </c>
-      <c r="F61" t="inlineStr"/>
-      <c r="G61" t="n">
+      <c r="G61">
         <v>-0.1904091039279596</v>
       </c>
-      <c r="H61" t="n">
+      <c r="H61">
         <v>0.07254116832879398</v>
       </c>
-      <c r="I61" t="n">
+      <c r="I61">
         <v>-0.1712693200335786</v>
       </c>
-      <c r="J61" t="n">
+      <c r="J61">
         <v>-0.07113312426889529</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" s="2" t="n">
+    <row r="62" spans="1:10">
+      <c r="A62" s="2">
         <v>39722</v>
       </c>
-      <c r="B62" t="n">
+      <c r="B62">
         <v>-0.3004455722744439</v>
       </c>
-      <c r="C62" t="n">
+      <c r="C62">
         <v>-0.323785320802374</v>
       </c>
-      <c r="D62" t="n">
+      <c r="D62">
         <v>-0.1021431128842515</v>
       </c>
-      <c r="E62" t="n">
+      <c r="E62">
         <v>0.04353225190176824</v>
       </c>
-      <c r="F62" t="inlineStr"/>
-      <c r="G62" t="n">
+      <c r="G62">
         <v>-0.2829711782132676</v>
       </c>
-      <c r="H62" t="n">
+      <c r="H62">
         <v>-0.1003086881760514</v>
       </c>
-      <c r="I62" t="n">
+      <c r="I62">
         <v>-0.5144606400965284</v>
       </c>
-      <c r="J62" t="n">
+      <c r="J62">
         <v>-0.3476415737641126</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" s="2" t="n">
+    <row r="63" spans="1:10">
+      <c r="A63" s="2">
         <v>39814</v>
       </c>
-      <c r="B63" t="n">
+      <c r="B63">
         <v>-0.063118948883231</v>
       </c>
-      <c r="C63" t="n">
+      <c r="C63">
         <v>-0.2209459536876841</v>
       </c>
-      <c r="D63" t="n">
+      <c r="D63">
         <v>0.008545060954768147</v>
       </c>
-      <c r="E63" t="n">
+      <c r="E63">
         <v>0.006232888681773074</v>
       </c>
-      <c r="F63" t="inlineStr"/>
-      <c r="G63" t="n">
+      <c r="G63">
         <v>0.03272603796412366</v>
       </c>
-      <c r="H63" t="n">
+      <c r="H63">
         <v>-0.03629763952182596</v>
       </c>
-      <c r="I63" t="n">
+      <c r="I63">
         <v>-0.246866802681434</v>
       </c>
-      <c r="J63" t="n">
+      <c r="J63">
         <v>-0.1607873473200303</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" s="2" t="n">
+    <row r="64" spans="1:10">
+      <c r="A64" s="2">
         <v>39904</v>
       </c>
-      <c r="B64" t="n">
+      <c r="B64">
         <v>0.1166694690727974</v>
       </c>
-      <c r="C64" t="n">
+      <c r="C64">
         <v>0.3590563803893021</v>
       </c>
-      <c r="D64" t="n">
+      <c r="D64">
         <v>0.06266945323090822</v>
       </c>
-      <c r="E64" t="n">
+      <c r="E64">
         <v>-0.0299293736251014</v>
       </c>
-      <c r="F64" t="inlineStr"/>
-      <c r="G64" t="n">
+      <c r="G64">
         <v>0.2613286990966428</v>
       </c>
-      <c r="H64" t="n">
+      <c r="H64">
         <v>0.003211355824285</v>
       </c>
-      <c r="I64" t="n">
+      <c r="I64">
         <v>0.5607177774156755</v>
       </c>
-      <c r="J64" t="n">
+      <c r="J64">
         <v>0.2765921198124366</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" s="2" t="n">
+    <row r="65" spans="1:10">
+      <c r="A65" s="2">
         <v>39995</v>
       </c>
-      <c r="B65" t="n">
+      <c r="B65">
         <v>0.04245041144057105</v>
       </c>
-      <c r="C65" t="n">
+      <c r="C65">
         <v>0.2508197430930557</v>
       </c>
-      <c r="D65" t="n">
+      <c r="D65">
         <v>0.07268716613070403</v>
       </c>
-      <c r="E65" t="n">
+      <c r="E65">
         <v>0.01765573449049018</v>
       </c>
-      <c r="F65" t="inlineStr"/>
-      <c r="G65" t="n">
+      <c r="G65">
         <v>0.03701550463391468</v>
       </c>
-      <c r="H65" t="n">
+      <c r="H65">
         <v>0.05617419643250954</v>
       </c>
-      <c r="I65" t="n">
+      <c r="I65">
         <v>0.307836867862969</v>
       </c>
-      <c r="J65" t="n">
+      <c r="J65">
         <v>0.135517196220476</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" s="2" t="n">
+    <row r="66" spans="1:10">
+      <c r="A66" s="2">
         <v>40087</v>
       </c>
-      <c r="B66" t="n">
+      <c r="B66">
         <v>0.09028158951876408</v>
       </c>
-      <c r="C66" t="n">
+      <c r="C66">
         <v>0.04395485553858869</v>
       </c>
-      <c r="D66" t="n">
+      <c r="D66">
         <v>0.03136613646499176</v>
       </c>
-      <c r="E66" t="n">
+      <c r="E66">
         <v>0.01057217056211779</v>
       </c>
-      <c r="F66" t="inlineStr"/>
-      <c r="G66" t="n">
+      <c r="G66">
         <v>0.05903854942800324</v>
       </c>
-      <c r="H66" t="n">
+      <c r="H66">
         <v>0.03320342957401956</v>
       </c>
-      <c r="I66" t="n">
+      <c r="I66">
         <v>-0.009210381886581631</v>
       </c>
-      <c r="J66" t="n">
+      <c r="J66">
         <v>0.03833457948710506</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" s="2" t="n">
+    <row r="67" spans="1:10">
+      <c r="A67" s="2">
         <v>40179</v>
       </c>
-      <c r="B67" t="n">
+      <c r="B67">
         <v>-0.05030132960277356</v>
       </c>
-      <c r="C67" t="n">
+      <c r="C67">
         <v>0.03965524385695929</v>
       </c>
-      <c r="D67" t="n">
+      <c r="D67">
         <v>0.03089266839627181</v>
       </c>
-      <c r="E67" t="n">
+      <c r="E67">
         <v>0.03578652430532525</v>
       </c>
-      <c r="F67" t="inlineStr"/>
-      <c r="G67" t="n">
+      <c r="G67">
         <v>-0.01433030851043349</v>
       </c>
-      <c r="H67" t="n">
+      <c r="H67">
         <v>0.02726081314154216</v>
       </c>
-      <c r="I67" t="n">
+      <c r="I67">
         <v>0.1237284721522813</v>
       </c>
-      <c r="J67" t="n">
+      <c r="J67">
         <v>-0.05863635500455811</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" s="2" t="n">
+    <row r="68" spans="1:10">
+      <c r="A68" s="2">
         <v>40269</v>
       </c>
-      <c r="B68" t="n">
+      <c r="B68">
         <v>-0.04811319047410778</v>
       </c>
-      <c r="C68" t="n">
+      <c r="C68">
         <v>-0.078864089278597</v>
       </c>
-      <c r="D68" t="n">
+      <c r="D68">
         <v>-0.02388497926084732</v>
       </c>
-      <c r="E68" t="n">
+      <c r="E68">
         <v>0.04469823688064722</v>
       </c>
-      <c r="F68" t="inlineStr"/>
-      <c r="G68" t="n">
+      <c r="G68">
         <v>0.01216861777832778</v>
       </c>
-      <c r="H68" t="n">
+      <c r="H68">
         <v>-0.00313083037910622</v>
       </c>
-      <c r="I68" t="n">
+      <c r="I68">
         <v>-0.148554783777728</v>
       </c>
-      <c r="J68" t="n">
+      <c r="J68">
         <v>-0.08112032312930828</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" s="2" t="n">
+    <row r="69" spans="1:10">
+      <c r="A69" s="2">
         <v>40360</v>
       </c>
-      <c r="B69" t="n">
+      <c r="B69">
         <v>0.1161153199770111</v>
       </c>
-      <c r="C69" t="n">
+      <c r="C69">
         <v>0.1844076274376605</v>
       </c>
-      <c r="D69" t="n">
+      <c r="D69">
         <v>0.05321206044546312</v>
       </c>
-      <c r="E69" t="n">
+      <c r="E69">
         <v>0.0290345810286976</v>
       </c>
-      <c r="F69" t="inlineStr"/>
-      <c r="G69" t="n">
+      <c r="G69">
         <v>0.04128549156395911</v>
       </c>
-      <c r="H69" t="n">
+      <c r="H69">
         <v>0.0542014470846901</v>
       </c>
-      <c r="I69" t="n">
+      <c r="I69">
         <v>0.2052947368421052</v>
       </c>
-      <c r="J69" t="n">
+      <c r="J69">
         <v>0.135988843771548</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" s="2" t="n">
+    <row r="70" spans="1:10">
+      <c r="A70" s="2">
         <v>40452</v>
       </c>
-      <c r="B70" t="n">
+      <c r="B70">
         <v>0.1579294590597877</v>
       </c>
-      <c r="C70" t="n">
+      <c r="C70">
         <v>0.06151272047111767</v>
       </c>
-      <c r="D70" t="n">
+      <c r="D70">
         <v>0.04687429167233326</v>
       </c>
-      <c r="E70" t="n">
+      <c r="E70">
         <v>-0.01806825288109348</v>
       </c>
-      <c r="F70" t="inlineStr"/>
-      <c r="G70" t="n">
+      <c r="G70">
         <v>0.05390514882641528</v>
       </c>
-      <c r="H70" t="n">
+      <c r="H70">
         <v>0.09944946398981225</v>
       </c>
-      <c r="I70" t="n">
+      <c r="I70">
         <v>0.1458302402557139</v>
       </c>
-      <c r="J70" t="n">
+      <c r="J70">
         <v>0.04391038157383398</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" s="2" t="n">
+    <row r="71" spans="1:10">
+      <c r="A71" s="2">
         <v>40544</v>
       </c>
-      <c r="B71" t="n">
+      <c r="B71">
         <v>0.04446875838026276</v>
       </c>
-      <c r="C71" t="n">
+      <c r="C71">
         <v>0.03043328629934283</v>
       </c>
-      <c r="D71" t="n">
+      <c r="D71">
         <v>0.0220629628025808</v>
       </c>
-      <c r="E71" t="n">
+      <c r="E71">
         <v>0.008188207464915775</v>
       </c>
-      <c r="F71" t="inlineStr"/>
-      <c r="G71" t="n">
+      <c r="G71">
         <v>0.0259183707213575</v>
       </c>
-      <c r="H71" t="n">
+      <c r="H71">
         <v>0.07645393924336896</v>
       </c>
-      <c r="I71" t="n">
+      <c r="I71">
         <v>0.08858926380134302</v>
       </c>
-      <c r="J71" t="n">
+      <c r="J71">
         <v>0.06783045143330724</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" s="2" t="n">
+    <row r="72" spans="1:10">
+      <c r="A72" s="2">
         <v>40634</v>
       </c>
-      <c r="B72" t="n">
+      <c r="B72">
         <v>-0.06725262626941375</v>
       </c>
-      <c r="C72" t="n">
+      <c r="C72">
         <v>0.02942090022811295</v>
       </c>
-      <c r="D72" t="n">
+      <c r="D72">
         <v>-0.005444338523461489</v>
       </c>
-      <c r="E72" t="n">
+      <c r="E72">
         <v>0.03141896718981485</v>
       </c>
-      <c r="F72" t="inlineStr"/>
-      <c r="G72" t="n">
+      <c r="G72">
         <v>0.03236295644215637</v>
       </c>
-      <c r="H72" t="n">
+      <c r="H72">
         <v>0.04993759125717578</v>
       </c>
-      <c r="I72" t="n">
+      <c r="I72">
         <v>-0.008983084075505521</v>
       </c>
-      <c r="J72" t="n">
+      <c r="J72">
         <v>0.06900865726707117</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" s="2" t="n">
+    <row r="73" spans="1:10">
+      <c r="A73" s="2">
         <v>40725</v>
       </c>
-      <c r="B73" t="n">
+      <c r="B73">
         <v>-0.1133297847976705</v>
       </c>
-      <c r="C73" t="n">
+      <c r="C73">
         <v>-0.1730116604265756</v>
       </c>
-      <c r="D73" t="n">
+      <c r="D73">
         <v>-0.0477549629377183</v>
       </c>
-      <c r="E73" t="n">
+      <c r="E73">
         <v>0.04573657540738574</v>
       </c>
-      <c r="F73" t="inlineStr"/>
-      <c r="G73" t="n">
+      <c r="G73">
         <v>-0.02445070077556766</v>
       </c>
-      <c r="H73" t="n">
+      <c r="H73">
         <v>-0.03080454865454785</v>
       </c>
-      <c r="I73" t="n">
+      <c r="I73">
         <v>-0.2801591058421236</v>
       </c>
-      <c r="J73" t="n">
+      <c r="J73">
         <v>-0.1547936492618124</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" s="2" t="n">
+    <row r="74" spans="1:10">
+      <c r="A74" s="2">
         <v>40817</v>
       </c>
-      <c r="B74" t="n">
+      <c r="B74">
         <v>0.003451804240940159</v>
       </c>
-      <c r="C74" t="n">
+      <c r="C74">
         <v>0.0736300295022283</v>
       </c>
-      <c r="D74" t="n">
+      <c r="D74">
         <v>0.007090770813761083</v>
       </c>
-      <c r="E74" t="n">
+      <c r="E74">
         <v>0.01971721002872528</v>
       </c>
-      <c r="F74" t="inlineStr"/>
-      <c r="G74" t="n">
+      <c r="G74">
         <v>0.03008883598997847</v>
       </c>
-      <c r="H74" t="n">
+      <c r="H74">
         <v>0.06102637624224228</v>
       </c>
-      <c r="I74" t="n">
+      <c r="I74">
         <v>0.0436463925721633</v>
       </c>
-      <c r="J74" t="n">
+      <c r="J74">
         <v>0.0005158853937901053</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" s="2" t="n">
+    <row r="75" spans="1:10">
+      <c r="A75" s="2">
         <v>40909</v>
       </c>
-      <c r="B75" t="n">
+      <c r="B75">
         <v>0.008850687084439146</v>
       </c>
-      <c r="C75" t="n">
+      <c r="C75">
         <v>0.1289720240879328</v>
       </c>
-      <c r="D75" t="n">
+      <c r="D75">
         <v>0.04035715078959634</v>
       </c>
-      <c r="E75" t="n">
+      <c r="E75">
         <v>-0.01467290230828144</v>
       </c>
-      <c r="F75" t="inlineStr"/>
-      <c r="G75" t="n">
+      <c r="G75">
         <v>0.04780016568835332</v>
       </c>
-      <c r="H75" t="n">
+      <c r="H75">
         <v>0.05565462153842016</v>
       </c>
-      <c r="I75" t="n">
+      <c r="I75">
         <v>0.177986344913198</v>
       </c>
-      <c r="J75" t="n">
+      <c r="J75">
         <v>0.1027457610550666</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" s="2" t="n">
+    <row r="76" spans="1:10">
+      <c r="A76" s="2">
         <v>41000</v>
       </c>
-      <c r="B76" t="n">
+      <c r="B76">
         <v>-0.04546335507083599</v>
       </c>
-      <c r="C76" t="n">
+      <c r="C76">
         <v>0.0211775672500234</v>
       </c>
-      <c r="D76" t="n">
+      <c r="D76">
         <v>-0.01763450042698544</v>
       </c>
-      <c r="E76" t="n">
+      <c r="E76">
         <v>0.04845604052459929</v>
       </c>
-      <c r="F76" t="inlineStr"/>
-      <c r="G76" t="n">
+      <c r="G76">
         <v>-0.01047490979040144</v>
       </c>
-      <c r="H76" t="n">
+      <c r="H76">
         <v>-0.02335597152789293</v>
       </c>
-      <c r="I76" t="n">
+      <c r="I76">
         <v>-0.06105700143701098</v>
       </c>
-      <c r="J76" t="n">
+      <c r="J76">
         <v>0.004535085040392239</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" s="2" t="n">
+    <row r="77" spans="1:10">
+      <c r="A77" s="2">
         <v>41091</v>
       </c>
-      <c r="B77" t="n">
+      <c r="B77">
         <v>0.09690417015626918</v>
       </c>
-      <c r="C77" t="n">
+      <c r="C77">
         <v>0.05505828806156532</v>
       </c>
-      <c r="D77" t="n">
+      <c r="D77">
         <v>0.03338114486895294</v>
       </c>
-      <c r="E77" t="n">
+      <c r="E77">
         <v>0.02477282203675868</v>
       </c>
-      <c r="F77" t="inlineStr"/>
-      <c r="G77" t="n">
+      <c r="G77">
         <v>0.07123715109295214</v>
       </c>
-      <c r="H77" t="n">
+      <c r="H77">
         <v>-0.008394252748809006</v>
       </c>
-      <c r="I77" t="n">
+      <c r="I77">
         <v>0.09717545828656959</v>
       </c>
-      <c r="J77" t="n">
+      <c r="J77">
         <v>0.06995695805709423</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" s="2" t="n">
+    <row r="78" spans="1:10">
+      <c r="A78" s="2">
         <v>41183</v>
       </c>
-      <c r="B78" t="n">
+      <c r="B78">
         <v>-0.06330728249648854</v>
       </c>
-      <c r="C78" t="n">
+      <c r="C78">
         <v>0.05767064315820147</v>
       </c>
-      <c r="D78" t="n">
+      <c r="D78">
         <v>0.01951629863301774</v>
       </c>
-      <c r="E78" t="n">
+      <c r="E78">
         <v>-0.0004973003694230815</v>
       </c>
-      <c r="F78" t="inlineStr"/>
-      <c r="G78" t="n">
+      <c r="G78">
         <v>0.02850164706003722</v>
       </c>
-      <c r="H78" t="n">
+      <c r="H78">
         <v>0.03563903712480565</v>
       </c>
-      <c r="I78" t="n">
+      <c r="I78">
         <v>0.07871994172394814</v>
       </c>
-      <c r="J78" t="n">
+      <c r="J78">
         <v>0.06024346886989096</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" s="2" t="n">
+    <row r="79" spans="1:10">
+      <c r="A79" s="2">
         <v>41275</v>
       </c>
-      <c r="B79" t="n">
+      <c r="B79">
         <v>-0.01125729980610102</v>
       </c>
-      <c r="C79" t="n">
+      <c r="C79">
         <v>0.06260970829664569</v>
       </c>
-      <c r="D79" t="n">
+      <c r="D79">
         <v>0.03550063946532456</v>
       </c>
-      <c r="E79" t="n">
+      <c r="E79">
         <v>0.02146563366266263</v>
       </c>
-      <c r="F79" t="inlineStr"/>
-      <c r="G79" t="n">
+      <c r="G79">
         <v>-0.01274557864067527</v>
       </c>
-      <c r="H79" t="n">
+      <c r="H79">
         <v>0.01863559818913019</v>
       </c>
-      <c r="I79" t="n">
+      <c r="I79">
         <v>0.1304792918919735</v>
       </c>
-      <c r="J79" t="n">
+      <c r="J79">
         <v>-0.044944705491481</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" s="2" t="n">
+    <row r="80" spans="1:10">
+      <c r="A80" s="2">
         <v>41365</v>
       </c>
-      <c r="B80" t="n">
+      <c r="B80">
         <v>-0.09451399781701997</v>
       </c>
-      <c r="C80" t="n">
+      <c r="C80">
         <v>-0.0362998733564458</v>
       </c>
-      <c r="D80" t="n">
+      <c r="D80">
         <v>0.001255005079782379</v>
       </c>
-      <c r="E80" t="n">
+      <c r="E80">
         <v>0.001448624439369661</v>
       </c>
-      <c r="F80" t="inlineStr"/>
-      <c r="G80" t="n">
+      <c r="G80">
         <v>0.03595519870904784</v>
       </c>
-      <c r="H80" t="n">
+      <c r="H80">
         <v>0.008619872654570315</v>
       </c>
-      <c r="I80" t="n">
+      <c r="I80">
         <v>0.0142213766119712</v>
       </c>
-      <c r="J80" t="n">
+      <c r="J80">
         <v>0.04349986100952763</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="2" t="n">
+    <row r="81" spans="1:10">
+      <c r="A81" s="2">
         <v>41456</v>
       </c>
-      <c r="B81" t="n">
+      <c r="B81">
         <v>0.02134030613650051</v>
       </c>
-      <c r="C81" t="n">
+      <c r="C81">
         <v>0.02439931861199662</v>
       </c>
-      <c r="D81" t="n">
+      <c r="D81">
         <v>0.01611555449444912</v>
       </c>
-      <c r="E81" t="n">
+      <c r="E81">
         <v>0.01931653085717899</v>
       </c>
-      <c r="F81" t="inlineStr"/>
-      <c r="G81" t="n">
+      <c r="G81">
         <v>0.05112258730432861</v>
       </c>
-      <c r="H81" t="n">
+      <c r="H81">
         <v>0.02547065533644965</v>
       </c>
-      <c r="I81" t="n">
+      <c r="I81">
         <v>0.1096531570254562</v>
       </c>
-      <c r="J81" t="n">
+      <c r="J81">
         <v>0.1090845763783885</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" s="2" t="n">
+    <row r="82" spans="1:10">
+      <c r="A82" s="2">
         <v>41548</v>
       </c>
-      <c r="B82" t="n">
+      <c r="B82">
         <v>-0.01053337908362373</v>
       </c>
-      <c r="C82" t="n">
+      <c r="C82">
         <v>-0.004893168119098124</v>
       </c>
-      <c r="D82" t="n">
+      <c r="D82">
         <v>0.04152960526315774</v>
       </c>
-      <c r="E82" t="n">
+      <c r="E82">
         <v>-0.008223439591492743</v>
       </c>
-      <c r="F82" t="inlineStr"/>
-      <c r="G82" t="n">
+      <c r="G82">
         <v>0.06491956620680917</v>
       </c>
-      <c r="H82" t="n">
+      <c r="H82">
         <v>0.02514070044882222</v>
       </c>
-      <c r="I82" t="n">
+      <c r="I82">
         <v>0.1081359591914635</v>
       </c>
-      <c r="J82" t="n">
+      <c r="J82">
         <v>0.07106031335204488</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" s="2" t="n">
+    <row r="83" spans="1:10">
+      <c r="A83" s="2">
         <v>41640</v>
       </c>
-      <c r="B83" t="n">
+      <c r="B83">
         <v>0.06989590677228041</v>
       </c>
-      <c r="C83" t="n">
+      <c r="C83">
         <v>0.04014413663019178</v>
       </c>
-      <c r="D83" t="n">
+      <c r="D83">
         <v>0.009343334649295931</v>
       </c>
-      <c r="E83" t="n">
+      <c r="E83">
         <v>0.04605694790709869</v>
       </c>
-      <c r="F83" t="inlineStr"/>
-      <c r="G83" t="n">
+      <c r="G83">
         <v>0.01514575679308972</v>
       </c>
-      <c r="H83" t="n">
+      <c r="H83">
         <v>0.007903455436109263</v>
       </c>
-      <c r="I83" t="n">
+      <c r="I83">
         <v>0.02565692625417126</v>
       </c>
-      <c r="J83" t="n">
+      <c r="J83">
         <v>0.05437403440759625</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" s="2" t="n">
+    <row r="84" spans="1:10">
+      <c r="A84" s="2">
         <v>41730</v>
       </c>
-      <c r="B84" t="n">
+      <c r="B84">
         <v>0.0008450136442570422</v>
       </c>
-      <c r="C84" t="n">
+      <c r="C84">
         <v>0.07875897624938277</v>
       </c>
-      <c r="D84" t="n">
+      <c r="D84">
         <v>0.01888619854721552</v>
       </c>
-      <c r="E84" t="n">
+      <c r="E84">
         <v>0.04470408333930664</v>
       </c>
-      <c r="F84" t="inlineStr"/>
-      <c r="G84" t="n">
+      <c r="G84">
         <v>0.07939124332287495</v>
       </c>
-      <c r="H84" t="n">
+      <c r="H84">
         <v>0.09900688663764257</v>
       </c>
-      <c r="I84" t="n">
+      <c r="I84">
         <v>0.0211266241169914</v>
       </c>
-      <c r="J84" t="n">
+      <c r="J84">
         <v>0.04131288868420024</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" s="2" t="n">
+    <row r="85" spans="1:10">
+      <c r="A85" s="2">
         <v>41821</v>
       </c>
-      <c r="B85" t="n">
+      <c r="B85">
         <v>-0.1183030930747835</v>
       </c>
-      <c r="C85" t="n">
+      <c r="C85">
         <v>-0.04433135298573754</v>
       </c>
-      <c r="D85" t="n">
+      <c r="D85">
         <v>0.005557180462123501</v>
       </c>
-      <c r="E85" t="n">
+      <c r="E85">
         <v>0.0190741926630682</v>
       </c>
-      <c r="F85" t="inlineStr"/>
-      <c r="G85" t="n">
+      <c r="G85">
         <v>-0.01549836292996898</v>
       </c>
-      <c r="H85" t="n">
+      <c r="H85">
         <v>0.02646508532748881</v>
       </c>
-      <c r="I85" t="n">
+      <c r="I85">
         <v>-0.08558092194758349</v>
       </c>
-      <c r="J85" t="n">
+      <c r="J85">
         <v>-0.03784008754296619</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" s="2" t="n">
+    <row r="86" spans="1:10">
+      <c r="A86" s="2">
         <v>41913</v>
       </c>
-      <c r="B86" t="n">
+      <c r="B86">
         <v>-0.1209615848814439</v>
       </c>
-      <c r="C86" t="n">
+      <c r="C86">
         <v>0.08073162147045831</v>
       </c>
-      <c r="D86" t="n">
+      <c r="D86">
         <v>0.00698080279232105</v>
       </c>
-      <c r="E86" t="n">
+      <c r="E86">
         <v>0.02334597603124022</v>
       </c>
-      <c r="F86" t="inlineStr"/>
-      <c r="G86" t="n">
+      <c r="G86">
         <v>0.01922130487953821</v>
       </c>
-      <c r="H86" t="n">
+      <c r="H86">
         <v>-0.118429876331218</v>
       </c>
-      <c r="I86" t="n">
+      <c r="I86">
         <v>0.0238730163459584</v>
       </c>
-      <c r="J86" t="n">
+      <c r="J86">
         <v>0.0275109556017008</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" s="2" t="n">
+    <row r="87" spans="1:10">
+      <c r="A87" s="2">
         <v>42005</v>
       </c>
-      <c r="B87" t="n">
+      <c r="B87">
         <v>-0.05942628217025925</v>
       </c>
-      <c r="C87" t="n">
+      <c r="C87">
         <v>0.04169564381944624</v>
       </c>
-      <c r="D87" t="n">
+      <c r="D87">
         <v>0.02482307914500281</v>
       </c>
-      <c r="E87" t="n">
+      <c r="E87">
         <v>0.04760599365107199</v>
       </c>
-      <c r="F87" t="inlineStr"/>
-      <c r="G87" t="n">
+      <c r="G87">
         <v>-0.01420436613344034</v>
       </c>
-      <c r="H87" t="n">
+      <c r="H87">
         <v>-0.05766319296915856</v>
       </c>
-      <c r="I87" t="n">
+      <c r="I87">
         <v>0.03660447266746525</v>
       </c>
-      <c r="J87" t="n">
+      <c r="J87">
         <v>0.01942622263175275</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" s="2" t="n">
+    <row r="88" spans="1:10">
+      <c r="A88" s="2">
         <v>42095</v>
       </c>
-      <c r="B88" t="n">
+      <c r="B88">
         <v>0.046581794023699</v>
       </c>
-      <c r="C88" t="n">
+      <c r="C88">
         <v>-0.06671548111596459</v>
       </c>
-      <c r="D88" t="n">
+      <c r="D88">
         <v>-0.004773900329416603</v>
       </c>
-      <c r="E88" t="n">
+      <c r="E88">
         <v>-0.0129948292825891</v>
       </c>
-      <c r="F88" t="inlineStr"/>
-      <c r="G88" t="n">
+      <c r="G88">
         <v>0.08587747188296024</v>
       </c>
-      <c r="H88" t="n">
+      <c r="H88">
         <v>-0.006680119035222254</v>
       </c>
-      <c r="I88" t="n">
+      <c r="I88">
         <v>0.03842249454204572</v>
       </c>
-      <c r="J88" t="n">
+      <c r="J88">
         <v>0.04921254973581513</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" s="2" t="n">
+    <row r="89" spans="1:10">
+      <c r="A89" s="2">
         <v>42186</v>
       </c>
-      <c r="B89" t="n">
+      <c r="B89">
         <v>-0.1446648578926299</v>
       </c>
-      <c r="C89" t="n">
+      <c r="C89">
         <v>-0.01421172915298685</v>
       </c>
-      <c r="D89" t="n">
+      <c r="D89">
         <v>-0.02525842537524781</v>
       </c>
-      <c r="E89" t="n">
+      <c r="E89">
         <v>0.01717455048702754</v>
       </c>
-      <c r="F89" t="inlineStr"/>
-      <c r="G89" t="n">
+      <c r="G89">
         <v>-0.04136995272218769</v>
       </c>
-      <c r="H89" t="n">
+      <c r="H89">
         <v>-0.0633756249646088</v>
       </c>
-      <c r="I89" t="n">
+      <c r="I89">
         <v>-0.09056115552465926</v>
       </c>
-      <c r="J89" t="n">
+      <c r="J89">
         <v>0.00241192680060287</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" s="2" t="n">
+    <row r="90" spans="1:10">
+      <c r="A90" s="2">
         <v>42278</v>
       </c>
-      <c r="B90" t="n">
+      <c r="B90">
         <v>-0.1051720376259181</v>
       </c>
-      <c r="C90" t="n">
+      <c r="C90">
         <v>0.04399562155746573</v>
       </c>
-      <c r="D90" t="n">
+      <c r="D90">
         <v>-0.001234814505438719</v>
       </c>
-      <c r="E90" t="n">
+      <c r="E90">
         <v>0.001459610492514196</v>
       </c>
-      <c r="F90" t="inlineStr"/>
-      <c r="G90" t="n">
+      <c r="G90">
         <v>0.0107478919131736</v>
       </c>
-      <c r="H90" t="n">
+      <c r="H90">
         <v>-0.06763480973741387</v>
       </c>
-      <c r="I90" t="n">
+      <c r="I90">
         <v>0.02250818537376698</v>
       </c>
-      <c r="J90" t="n">
+      <c r="J90">
         <v>-0.035495730813909</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" s="2" t="n">
+    <row r="91" spans="1:10">
+      <c r="A91" s="2">
         <v>42370</v>
       </c>
-      <c r="B91" t="n">
+      <c r="B91">
         <v>0.004164521661134346</v>
       </c>
-      <c r="C91" t="n">
+      <c r="C91">
         <v>0.05432659150090946</v>
       </c>
-      <c r="D91" t="n">
+      <c r="D91">
         <v>-0.02201778149488198</v>
       </c>
-      <c r="E91" t="n">
+      <c r="E91">
         <v>0.02791080203214791</v>
       </c>
-      <c r="F91" t="inlineStr"/>
-      <c r="G91" t="n">
+      <c r="G91">
         <v>0.01129195087134116</v>
       </c>
-      <c r="H91" t="n">
+      <c r="H91">
         <v>-0.04571470589023752</v>
       </c>
-      <c r="I91" t="n">
+      <c r="I91">
         <v>0.006376638546398361</v>
       </c>
-      <c r="J91" t="n">
+      <c r="J91">
         <v>-0.07016372229121703</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" s="2" t="n">
+    <row r="92" spans="1:10">
+      <c r="A92" s="2">
         <v>42461</v>
       </c>
-      <c r="B92" t="n">
+      <c r="B92">
         <v>0.1278111727289197</v>
       </c>
-      <c r="C92" t="n">
+      <c r="C92">
         <v>0.03743825366223796</v>
       </c>
-      <c r="D92" t="n">
+      <c r="D92">
         <v>0.00594906116378513</v>
       </c>
-      <c r="E92" t="n">
+      <c r="E92">
         <v>0.04052685416814361</v>
       </c>
-      <c r="F92" t="inlineStr"/>
-      <c r="G92" t="n">
+      <c r="G92">
         <v>-0.006681964135838325</v>
       </c>
-      <c r="H92" t="n">
+      <c r="H92">
         <v>0.07294388117421891</v>
       </c>
-      <c r="I92" t="n">
+      <c r="I92">
         <v>-0.0337430417743726</v>
       </c>
-      <c r="J92" t="n">
+      <c r="J92">
         <v>-0.1127645866596674</v>
       </c>
     </row>
-    <row r="93">
-      <c r="A93" s="2" t="n">
+    <row r="93" spans="1:10">
+      <c r="A93" s="2">
         <v>42552</v>
       </c>
-      <c r="B93" t="n">
+      <c r="B93">
         <v>-0.03863991169677516</v>
       </c>
-      <c r="C93" t="n">
+      <c r="C93">
         <v>0.01455639646255591</v>
       </c>
-      <c r="D93" t="n">
+      <c r="D93">
         <v>0.0174274625762334</v>
       </c>
-      <c r="E93" t="n">
+      <c r="E93">
         <v>0.02466456099709458</v>
       </c>
-      <c r="F93" t="inlineStr"/>
-      <c r="G93" t="n">
+      <c r="G93">
         <v>0.02212095186304563</v>
       </c>
-      <c r="H93" t="n">
+      <c r="H93">
         <v>0.05539564431099353</v>
       </c>
-      <c r="I93" t="n">
+      <c r="I93">
         <v>0.0929096411817496</v>
       </c>
-      <c r="J93" t="n">
+      <c r="J93">
         <v>0.008619609114524973</v>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" s="2" t="n">
+    <row r="94" spans="1:10">
+      <c r="A94" s="2">
         <v>42644</v>
       </c>
-      <c r="B94" t="n">
+      <c r="B94">
         <v>0.02656130793352429</v>
       </c>
-      <c r="C94" t="n">
+      <c r="C94">
         <v>-0.05394018997932593</v>
       </c>
-      <c r="D94" t="n">
+      <c r="D94">
         <v>0.01149801100757464</v>
       </c>
-      <c r="E94" t="n">
+      <c r="E94">
         <v>-0.02321119000688687</v>
       </c>
-      <c r="F94" t="inlineStr"/>
-      <c r="G94" t="n">
+      <c r="G94">
         <v>-0.05999239366822451</v>
       </c>
-      <c r="H94" t="n">
+      <c r="H94">
         <v>0.07366043663857358</v>
       </c>
-      <c r="I94" t="n">
+      <c r="I94">
         <v>0.02341008386284948</v>
       </c>
-      <c r="J94" t="n">
+      <c r="J94">
         <v>-0.04345655483799815</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" s="2" t="n">
+    <row r="95" spans="1:10">
+      <c r="A95" s="2">
         <v>42736</v>
       </c>
-      <c r="B95" t="n">
+      <c r="B95">
         <v>-0.02326133410044107</v>
       </c>
-      <c r="C95" t="n">
+      <c r="C95">
         <v>0.02296595464950091</v>
       </c>
-      <c r="D95" t="n">
+      <c r="D95">
         <v>0.02074129942894087</v>
       </c>
-      <c r="E95" t="n">
+      <c r="E95">
         <v>0.02135584319598571</v>
       </c>
-      <c r="F95" t="inlineStr"/>
-      <c r="G95" t="n">
+      <c r="G95">
         <v>0.03870305083038184</v>
       </c>
-      <c r="H95" t="n">
+      <c r="H95">
         <v>0.03604808443194685</v>
       </c>
-      <c r="I95" t="n">
+      <c r="I95">
         <v>0.07170861582109667</v>
       </c>
-      <c r="J95" t="n">
+      <c r="J95">
         <v>0.02599298974381381</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" s="2" t="n">
+    <row r="96" spans="1:10">
+      <c r="A96" s="2">
         <v>42826</v>
       </c>
-      <c r="B96" t="n">
+      <c r="B96">
         <v>-0.03000651523094344</v>
       </c>
-      <c r="C96" t="n">
+      <c r="C96">
         <v>0.03005506138059055</v>
       </c>
-      <c r="D96" t="n">
+      <c r="D96">
         <v>0.007582554845974032</v>
       </c>
-      <c r="E96" t="n">
+      <c r="E96">
         <v>0.01418233753868114</v>
       </c>
-      <c r="F96" t="inlineStr"/>
-      <c r="G96" t="n">
+      <c r="G96">
         <v>0.04888619827568452</v>
       </c>
-      <c r="H96" t="n">
+      <c r="H96">
         <v>-0.0004464816188188836</v>
       </c>
-      <c r="I96" t="n">
+      <c r="I96">
         <v>0.0939602576213272</v>
       </c>
-      <c r="J96" t="n">
+      <c r="J96">
         <v>0.06202735212324417</v>
       </c>
     </row>
-    <row r="97">
-      <c r="A97" s="2" t="n">
+    <row r="97" spans="1:10">
+      <c r="A97" s="2">
         <v>42917</v>
       </c>
-      <c r="B97" t="n">
+      <c r="B97">
         <v>0.0252022340743463</v>
       </c>
-      <c r="C97" t="n">
+      <c r="C97">
         <v>0.01839579745335684</v>
       </c>
-      <c r="D97" t="n">
+      <c r="D97">
         <v>0.01805419751361903</v>
       </c>
-      <c r="E97" t="n">
+      <c r="E97">
         <v>0.004924212196461664</v>
       </c>
-      <c r="F97" t="inlineStr"/>
-      <c r="G97" t="n">
+      <c r="G97">
         <v>0.037181043051429</v>
       </c>
-      <c r="H97" t="n">
+      <c r="H97">
         <v>0.02098379132088901</v>
       </c>
-      <c r="I97" t="n">
+      <c r="I97">
         <v>0.05740711262270093</v>
       </c>
-      <c r="J97" t="n">
+      <c r="J97">
         <v>0.03224412967233925</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" s="2" t="n">
+    <row r="98" spans="1:10">
+      <c r="A98" s="2">
         <v>43009</v>
       </c>
-      <c r="B98" t="n">
+      <c r="B98">
         <v>0.04708584887655887</v>
       </c>
-      <c r="C98" t="n">
+      <c r="C98">
         <v>0.03830529834597241</v>
       </c>
-      <c r="D98" t="n">
+      <c r="D98">
         <v>0.02303365005316782</v>
       </c>
-      <c r="E98" t="n">
+      <c r="E98">
         <v>-0.003545436709984306</v>
       </c>
-      <c r="F98" t="inlineStr"/>
-      <c r="G98" t="n">
+      <c r="G98">
         <v>0.0462976208188477</v>
       </c>
-      <c r="H98" t="n">
+      <c r="H98">
         <v>0.0262576857662371</v>
       </c>
-      <c r="I98" t="n">
+      <c r="I98">
         <v>0.01129562401411621</v>
       </c>
-      <c r="J98" t="n">
+      <c r="J98">
         <v>0.06983606216589244</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" s="2" t="n">
+    <row r="99" spans="1:10">
+      <c r="A99" s="2">
         <v>43101</v>
       </c>
-      <c r="B99" t="n">
+      <c r="B99">
         <v>-0.004007619589546874</v>
       </c>
-      <c r="C99" t="n">
+      <c r="C99">
         <v>-0.04304571120138145</v>
       </c>
-      <c r="D99" t="n">
+      <c r="D99">
         <v>0.004677362571040566</v>
       </c>
-      <c r="E99" t="n">
+      <c r="E99">
         <v>0.009389693370023267</v>
       </c>
-      <c r="F99" t="inlineStr"/>
-      <c r="G99" t="n">
+      <c r="G99">
         <v>-0.0540901839025254</v>
       </c>
-      <c r="H99" t="n">
+      <c r="H99">
         <v>0.01595719865195977</v>
       </c>
-      <c r="I99" t="n">
+      <c r="I99">
         <v>-0.0164686497169183</v>
       </c>
-      <c r="J99" t="n">
+      <c r="J99">
         <v>0.01272366417299642</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" s="2" t="n">
+    <row r="100" spans="1:10">
+      <c r="A100" s="2">
         <v>43191</v>
       </c>
-      <c r="B100" t="n">
+      <c r="B100">
         <v>0.004005333749916407</v>
       </c>
-      <c r="C100" t="n">
+      <c r="C100">
         <v>0.05450911016524729</v>
       </c>
-      <c r="D100" t="n">
+      <c r="D100">
         <v>0.0009678280603391265</v>
       </c>
-      <c r="E100" t="n">
+      <c r="E100">
         <v>0.0144806382998488</v>
       </c>
-      <c r="F100" t="inlineStr"/>
-      <c r="G100" t="n">
+      <c r="G100">
         <v>0.002852055095870831</v>
       </c>
-      <c r="H100" t="n">
+      <c r="H100">
         <v>0.03272213744257968</v>
       </c>
-      <c r="I100" t="n">
+      <c r="I100">
         <v>0.02449591038062682</v>
       </c>
-      <c r="J100" t="n">
+      <c r="J100">
         <v>-0.02395744516650899</v>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" s="2" t="n">
+    <row r="101" spans="1:10">
+      <c r="A101" s="2">
         <v>43282</v>
       </c>
-      <c r="B101" t="n">
+      <c r="B101">
         <v>-0.02023518245506217</v>
       </c>
-      <c r="C101" t="n">
+      <c r="C101">
         <v>-0.001540338401698982</v>
       </c>
-      <c r="D101" t="n">
+      <c r="D101">
         <v>0.00588470643150063</v>
       </c>
-      <c r="E101" t="n">
+      <c r="E101">
         <v>0.004783922358542414</v>
       </c>
-      <c r="F101" t="inlineStr"/>
-      <c r="G101" t="n">
+      <c r="G101">
         <v>0.06876661406457818</v>
       </c>
-      <c r="H101" t="n">
+      <c r="H101">
         <v>0.03372220608462517</v>
       </c>
-      <c r="I101" t="n">
+      <c r="I101">
         <v>0.05603607878935346</v>
       </c>
-      <c r="J101" t="n">
+      <c r="J101">
         <v>-0.04743689485986402</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" s="2" t="n">
+    <row r="102" spans="1:10">
+      <c r="A102" s="2">
         <v>43374</v>
       </c>
-      <c r="B102" t="n">
+      <c r="B102">
         <v>-0.09410733782346681</v>
       </c>
-      <c r="C102" t="n">
+      <c r="C102">
         <v>-0.05456374438773548</v>
       </c>
-      <c r="D102" t="n">
+      <c r="D102">
         <v>-0.04297386433318406</v>
       </c>
-      <c r="E102" t="n">
+      <c r="E102">
         <v>0.02111306011800362</v>
       </c>
-      <c r="F102" t="inlineStr"/>
-      <c r="G102" t="n">
+      <c r="G102">
         <v>0.02059662582274968</v>
       </c>
-      <c r="H102" t="n">
+      <c r="H102">
         <v>-0.03409336309653721</v>
       </c>
-      <c r="I102" t="n">
+      <c r="I102">
         <v>-0.1925083006554655</v>
       </c>
-      <c r="J102" t="n">
+      <c r="J102">
         <v>-0.08431752969050543</v>
       </c>
     </row>
-    <row r="103">
-      <c r="A103" s="2" t="n">
+    <row r="103" spans="1:10">
+      <c r="A103" s="2">
         <v>43466</v>
       </c>
-      <c r="B103" t="n">
+      <c r="B103">
         <v>0.06323871370058387</v>
       </c>
-      <c r="C103" t="n">
+      <c r="C103">
         <v>0.1485804645673736</v>
       </c>
-      <c r="D103" t="n">
+      <c r="D103">
         <v>0.03989886745402282</v>
       </c>
-      <c r="E103" t="n">
+      <c r="E103">
         <v>0.01580856598503466</v>
       </c>
-      <c r="F103" t="inlineStr"/>
-      <c r="G103" t="n">
+      <c r="G103">
         <v>0.04162321390293178</v>
       </c>
-      <c r="H103" t="n">
+      <c r="H103">
         <v>-0.01219576101388464</v>
       </c>
-      <c r="I103" t="n">
+      <c r="I103">
         <v>0.1444959849918495</v>
       </c>
-      <c r="J103" t="n">
+      <c r="J103">
         <v>0.1075504904365392</v>
       </c>
     </row>
-    <row r="104">
-      <c r="A104" s="2" t="n">
+    <row r="104" spans="1:10">
+      <c r="A104" s="2">
         <v>43556</v>
       </c>
-      <c r="B104" t="n">
+      <c r="B104">
         <v>-0.01187723286972664</v>
       </c>
-      <c r="C104" t="n">
+      <c r="C104">
         <v>0.002021845819779378</v>
       </c>
-      <c r="D104" t="n">
+      <c r="D104">
         <v>0.02349708576186504</v>
       </c>
-      <c r="E104" t="n">
+      <c r="E104">
         <v>0.03676502885857125</v>
       </c>
-      <c r="F104" t="inlineStr"/>
-      <c r="G104" t="n">
+      <c r="G104">
         <v>0.02036099474413477</v>
       </c>
-      <c r="H104" t="n">
+      <c r="H104">
         <v>-0.02963757641763487</v>
       </c>
-      <c r="I104" t="n">
+      <c r="I104">
         <v>0.105406034252141</v>
       </c>
-      <c r="J104" t="n">
+      <c r="J104">
         <v>-0.03915295887676729</v>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" s="2" t="n">
+    <row r="105" spans="1:10">
+      <c r="A105" s="2">
         <v>43647</v>
       </c>
-      <c r="B105" t="n">
+      <c r="B105">
         <v>-0.0183684865113225</v>
       </c>
-      <c r="C105" t="n">
+      <c r="C105">
         <v>0.04866827185444866</v>
       </c>
-      <c r="D105" t="n">
+      <c r="D105">
         <v>0.002619547355233509</v>
       </c>
-      <c r="E105" t="n">
+      <c r="E105">
         <v>0.03715174213665939</v>
       </c>
-      <c r="F105" t="inlineStr"/>
-      <c r="G105" t="n">
+      <c r="G105">
         <v>0.001110639442982508</v>
       </c>
-      <c r="H105" t="n">
+      <c r="H105">
         <v>-0.03146814167644918</v>
       </c>
-      <c r="I105" t="n">
+      <c r="I105">
         <v>0.03162834419096927</v>
       </c>
-      <c r="J105" t="n">
+      <c r="J105">
         <v>0.01614289356379084</v>
       </c>
     </row>
-    <row r="106">
-      <c r="A106" s="2" t="n">
+    <row r="106" spans="1:10">
+      <c r="A106" s="2">
         <v>43739</v>
       </c>
-      <c r="B106" t="n">
+      <c r="B106">
         <v>0.04421283451937641</v>
       </c>
-      <c r="C106" t="n">
+      <c r="C106">
         <v>0.01964168462391447</v>
       </c>
-      <c r="D106" t="n">
+      <c r="D106">
         <v>0.02437441173606825</v>
       </c>
-      <c r="E106" t="n">
+      <c r="E106">
         <v>-0.009742607260591396</v>
       </c>
-      <c r="F106" t="inlineStr"/>
-      <c r="G106" t="n">
+      <c r="G106">
         <v>0.128995062447506</v>
       </c>
-      <c r="H106" t="n">
+      <c r="H106">
         <v>-0.01802238787235921</v>
       </c>
-      <c r="I106" t="n">
+      <c r="I106">
         <v>0.09397456201548415</v>
       </c>
-      <c r="J106" t="n">
+      <c r="J106">
         <v>0.1718247552643533</v>
       </c>
     </row>
-    <row r="107">
-      <c r="A107" s="2" t="n">
+    <row r="107" spans="1:10">
+      <c r="A107" s="2">
         <v>43831</v>
       </c>
-      <c r="B107" t="n">
+      <c r="B107">
         <v>-0.2329495442553147</v>
       </c>
-      <c r="C107" t="n">
+      <c r="C107">
         <v>-0.2833523049677126</v>
       </c>
-      <c r="D107" t="n">
+      <c r="D107">
         <v>-0.08982320512008113</v>
       </c>
-      <c r="E107" t="n">
+      <c r="E107">
         <v>0.01937578377664861</v>
       </c>
-      <c r="F107" t="inlineStr"/>
-      <c r="G107" t="n">
+      <c r="G107">
         <v>-0.1470150557516529</v>
       </c>
-      <c r="H107" t="n">
+      <c r="H107">
         <v>-0.2197283278931813</v>
       </c>
-      <c r="I107" t="n">
+      <c r="I107">
         <v>-0.3204313795344224</v>
       </c>
-      <c r="J107" t="n">
+      <c r="J107">
         <v>-0.2469500375114132</v>
       </c>
     </row>
-    <row r="108">
-      <c r="A108" s="2" t="n">
+    <row r="108" spans="1:10">
+      <c r="A108" s="2">
         <v>43922</v>
       </c>
-      <c r="B108" t="n">
+      <c r="B108">
         <v>0.05079966862696206</v>
       </c>
-      <c r="C108" t="n">
+      <c r="C108">
         <v>0.1032996746707124</v>
       </c>
-      <c r="D108" t="n">
+      <c r="D108">
         <v>0.06196261356911625</v>
       </c>
-      <c r="E108" t="n">
+      <c r="E108">
         <v>0.01872827410941547</v>
       </c>
-      <c r="F108" t="inlineStr"/>
-      <c r="G108" t="n">
+      <c r="G108">
         <v>0.1259300777996835</v>
       </c>
-      <c r="H108" t="n">
+      <c r="H108">
         <v>0.0134330932235085</v>
       </c>
-      <c r="I108" t="n">
+      <c r="I108">
         <v>0.2631527513806908</v>
       </c>
-      <c r="J108" t="n">
+      <c r="J108">
         <v>0.03190003033104549</v>
       </c>
     </row>
-    <row r="109">
-      <c r="A109" s="2" t="n">
+    <row r="109" spans="1:10">
+      <c r="A109" s="2">
         <v>44013</v>
       </c>
-      <c r="B109" t="n">
+      <c r="B109">
         <v>0.09074483078978224</v>
       </c>
-      <c r="C109" t="n">
+      <c r="C109">
         <v>0.02325776936459922</v>
       </c>
-      <c r="D109" t="n">
+      <c r="D109">
         <v>0.03435277149506666</v>
       </c>
-      <c r="E109" t="n">
+      <c r="E109">
         <v>0.01416535248529249</v>
       </c>
-      <c r="F109" t="inlineStr"/>
-      <c r="G109" t="n">
+      <c r="G109">
         <v>0.02338309215474244</v>
       </c>
-      <c r="H109" t="n">
+      <c r="H109">
         <v>0.01230810116153314</v>
       </c>
-      <c r="I109" t="n">
+      <c r="I109">
         <v>0.03323982054220531</v>
       </c>
-      <c r="J109" t="n">
+      <c r="J109">
         <v>0.02686447327013552</v>
       </c>
     </row>
-    <row r="110">
-      <c r="A110" s="2" t="n">
+    <row r="110" spans="1:10">
+      <c r="A110" s="2">
         <v>44105</v>
       </c>
-      <c r="B110" t="n">
+      <c r="B110">
         <v>0.1019191384145766</v>
       </c>
-      <c r="C110" t="n">
+      <c r="C110">
         <v>0.1348638726838631</v>
       </c>
-      <c r="D110" t="n">
+      <c r="D110">
         <v>0.06385675804151481</v>
       </c>
-      <c r="E110" t="n">
+      <c r="E110">
         <v>0.0108457660777026</v>
       </c>
-      <c r="F110" t="inlineStr"/>
-      <c r="G110" t="n">
+      <c r="G110">
         <v>0.1277689243294151</v>
       </c>
-      <c r="H110" t="n">
+      <c r="H110">
         <v>0.02908313728900058</v>
       </c>
-      <c r="I110" t="n">
+      <c r="I110">
         <v>0.2470589264377347</v>
       </c>
-      <c r="J110" t="n">
+      <c r="J110">
         <v>0.1575576244000658</v>
       </c>
     </row>
-    <row r="111">
-      <c r="A111" s="2" t="n">
+    <row r="111" spans="1:10">
+      <c r="A111" s="2">
         <v>44197</v>
       </c>
-      <c r="B111" t="n">
+      <c r="B111">
         <v>0.06920200922997521</v>
       </c>
-      <c r="C111" t="n">
+      <c r="C111">
         <v>0.0610938090693538</v>
       </c>
-      <c r="D111" t="n">
+      <c r="D111">
         <v>0.02853738456955601</v>
       </c>
-      <c r="E111" t="n">
+      <c r="E111">
         <v>-0.03750058122413558</v>
       </c>
-      <c r="F111" t="inlineStr"/>
-      <c r="G111" t="n">
+      <c r="G111">
         <v>-0.01886070133455908</v>
       </c>
-      <c r="H111" t="n">
+      <c r="H111">
         <v>0.08202462858383641</v>
       </c>
-      <c r="I111" t="n">
+      <c r="I111">
         <v>0.1279649668098795</v>
       </c>
-      <c r="J111" t="n">
+      <c r="J111">
         <v>0.03163765761163861</v>
       </c>
     </row>
-    <row r="112">
-      <c r="A112" s="2" t="n">
+    <row r="112" spans="1:10">
+      <c r="A112" s="2">
         <v>44287</v>
       </c>
-      <c r="B112" t="n">
+      <c r="B112">
         <v>0.1330473018406821</v>
       </c>
-      <c r="C112" t="n">
+      <c r="C112">
         <v>0.09421418115830682</v>
       </c>
-      <c r="D112" t="n">
+      <c r="D112">
         <v>0.03022184893419833</v>
       </c>
-      <c r="E112" t="n">
+      <c r="E112">
         <v>0.02051948888477351</v>
       </c>
-      <c r="F112" t="inlineStr"/>
-      <c r="G112" t="n">
+      <c r="G112">
         <v>0.01774519674422015</v>
       </c>
-      <c r="H112" t="n">
+      <c r="H112">
         <v>0.111440129335032</v>
       </c>
-      <c r="I112" t="n">
+      <c r="I112">
         <v>0.1670164375308902</v>
       </c>
-      <c r="J112" t="n">
+      <c r="J112">
         <v>0.05656504755150515</v>
       </c>
     </row>
-    <row r="113">
-      <c r="A113" s="2" t="n">
+    <row r="113" spans="1:10">
+      <c r="A113" s="2">
         <v>44378</v>
       </c>
-      <c r="B113" t="n">
+      <c r="B113">
         <v>0.06589067411978844</v>
       </c>
-      <c r="C113" t="n">
+      <c r="C113">
         <v>-0.007264006885975727</v>
       </c>
-      <c r="D113" t="n">
+      <c r="D113">
         <v>0.01191965477980972</v>
       </c>
-      <c r="E113" t="n">
+      <c r="E113">
         <v>0.003692380520325944</v>
       </c>
-      <c r="F113" t="inlineStr"/>
-      <c r="G113" t="n">
+      <c r="G113">
         <v>-0.01495565534953858</v>
       </c>
-      <c r="H113" t="n">
+      <c r="H113">
         <v>0.05000902755679459</v>
       </c>
-      <c r="I113" t="n">
+      <c r="I113">
         <v>0.04381973353363033</v>
       </c>
-      <c r="J113" t="n">
+      <c r="J113">
         <v>0.009733377719178815</v>
       </c>
     </row>
-    <row r="114">
-      <c r="A114" s="2" t="n">
+    <row r="114" spans="1:10">
+      <c r="A114" s="2">
         <v>44470</v>
       </c>
-      <c r="B114" t="n">
+      <c r="B114">
         <v>-0.01563434592524049</v>
       </c>
-      <c r="C114" t="n">
+      <c r="C114">
         <v>0.1036864131937976</v>
       </c>
-      <c r="D114" t="n">
+      <c r="D114">
         <v>0.009376172021502649</v>
       </c>
-      <c r="E114" t="n">
+      <c r="E114">
         <v>-0.003600190228391975</v>
       </c>
-      <c r="F114" t="inlineStr"/>
-      <c r="G114" t="n">
+      <c r="G114">
         <v>0.1075331844319212</v>
       </c>
-      <c r="H114" t="n">
+      <c r="H114">
         <v>0.06012746873259567</v>
       </c>
-      <c r="I114" t="n">
+      <c r="I114">
         <v>0.1021265239046591</v>
       </c>
-      <c r="J114" t="n">
+      <c r="J114">
         <v>0.08603273755999519</v>
       </c>
     </row>
-    <row r="115">
-      <c r="A115" s="2" t="n">
+    <row r="115" spans="1:10">
+      <c r="A115" s="2">
         <v>44562</v>
       </c>
-      <c r="B115" t="n">
+      <c r="B115">
         <v>0.2554747730559439</v>
       </c>
-      <c r="C115" t="n">
+      <c r="C115">
         <v>-0.03768565689222425</v>
       </c>
-      <c r="D115" t="n">
+      <c r="D115">
         <v>0.02134423251589457</v>
       </c>
-      <c r="E115" t="n">
+      <c r="E115">
         <v>-0.05871841902845987</v>
       </c>
-      <c r="F115" t="n">
+      <c r="F115">
         <v>0.0747044234781582</v>
       </c>
-      <c r="G115" t="n">
+      <c r="G115">
         <v>-0.02314811372385994</v>
       </c>
-      <c r="H115" t="n">
+      <c r="H115">
         <v>0.1061560530908428</v>
       </c>
-      <c r="I115" t="n">
+      <c r="I115">
         <v>-0.1162260342003444</v>
       </c>
-      <c r="J115" t="n">
+      <c r="J115">
         <v>-0.04750637182048956</v>
       </c>
     </row>
-    <row r="116">
-      <c r="A116" s="2" t="n">
+    <row r="116" spans="1:10">
+      <c r="A116" s="2">
         <v>44652</v>
       </c>
-      <c r="B116" t="n">
+      <c r="B116">
         <v>-0.05663040302173228</v>
       </c>
-      <c r="C116" t="n">
+      <c r="C116">
         <v>-0.1723319960326773</v>
       </c>
-      <c r="D116" t="n">
+      <c r="D116">
         <v>-0.0229731732621905</v>
       </c>
-      <c r="E116" t="n">
+      <c r="E116">
         <v>-0.04968381881498052</v>
       </c>
-      <c r="F116" t="n">
+      <c r="F116">
         <v>-0.07423992673992674</v>
       </c>
-      <c r="G116" t="n">
+      <c r="G116">
         <v>-0.102697357787606</v>
       </c>
-      <c r="H116" t="n">
+      <c r="H116">
         <v>0.06387765943484602</v>
       </c>
-      <c r="I116" t="n">
+      <c r="I116">
         <v>-0.2426609119414253</v>
       </c>
-      <c r="J116" t="n">
+      <c r="J116">
         <v>-0.1851181967539315</v>
       </c>
     </row>
-    <row r="117">
-      <c r="A117" s="2" t="n">
+    <row r="117" spans="1:10">
+      <c r="A117" s="2">
         <v>44743</v>
       </c>
-      <c r="B117" t="n">
+      <c r="B117">
         <v>-0.04107155172173238</v>
       </c>
-      <c r="C117" t="n">
+      <c r="C117">
         <v>-0.1138675999115685</v>
       </c>
-      <c r="D117" t="n">
+      <c r="D117">
         <v>0.003530450132391838</v>
       </c>
-      <c r="E117" t="n">
+      <c r="E117">
         <v>-0.0639097247026762</v>
       </c>
-      <c r="F117" t="n">
+      <c r="F117">
         <v>-0.09635681995786061</v>
       </c>
-      <c r="G117" t="n">
+      <c r="G117">
         <v>-0.1380623418662745</v>
       </c>
-      <c r="H117" t="n">
+      <c r="H117">
         <v>0.03685246604462655</v>
       </c>
-      <c r="I117" t="n">
+      <c r="I117">
         <v>-0.09362175059998512</v>
       </c>
-      <c r="J117" t="n">
+      <c r="J117">
         <v>-0.2067644978708145</v>
       </c>
     </row>
-    <row r="118">
-      <c r="A118" s="2" t="n">
+    <row r="118" spans="1:10">
+      <c r="A118" s="2">
         <v>44835</v>
       </c>
-      <c r="B118" t="n">
+      <c r="B118">
         <v>0.0221877274717015</v>
       </c>
-      <c r="C118" t="n">
+      <c r="C118">
         <v>0.07106898979656817</v>
       </c>
-      <c r="D118" t="n">
+      <c r="D118">
         <v>0.008176671064204166</v>
       </c>
-      <c r="E118" t="n">
+      <c r="E118">
         <v>0.02394007914075735</v>
       </c>
-      <c r="F118" t="n">
+      <c r="F118">
         <v>0.1103588317716089</v>
       </c>
-      <c r="G118" t="n">
+      <c r="G118">
         <v>0.1392857492753905</v>
       </c>
-      <c r="H118" t="n">
+      <c r="H118">
         <v>0.03188742893054175</v>
       </c>
-      <c r="I118" t="n">
+      <c r="I118">
         <v>0.1358443280591428</v>
       </c>
-      <c r="J118" t="n">
+      <c r="J118">
         <v>0.1185313894486375</v>
       </c>
     </row>
-    <row r="119">
-      <c r="A119" s="2" t="n">
+    <row r="119" spans="1:10">
+      <c r="A119" s="2">
         <v>44927</v>
       </c>
-      <c r="B119" t="n">
+      <c r="B119">
         <v>-0.05361235873718728</v>
       </c>
-      <c r="C119" t="n">
+      <c r="C119">
         <v>0.01035882483165307</v>
       </c>
-      <c r="D119" t="n">
+      <c r="D119">
         <v>0.002603492223600457</v>
       </c>
-      <c r="E119" t="n">
+      <c r="E119">
         <v>0.03101738114297814</v>
       </c>
-      <c r="F119" t="n">
+      <c r="F119">
         <v>0.0393804808076228</v>
       </c>
-      <c r="G119" t="n">
+      <c r="G119">
         <v>-0.03123301510564491</v>
       </c>
-      <c r="H119" t="n">
+      <c r="H119">
         <v>0.001511099673913385</v>
       </c>
-      <c r="I119" t="n">
+      <c r="I119">
         <v>0.06918249139998145</v>
       </c>
-      <c r="J119" t="n">
+      <c r="J119">
         <v>0.01982733277834248</v>
       </c>
     </row>
-    <row r="120">
-      <c r="A120" s="2" t="n">
+    <row r="120" spans="1:10">
+      <c r="A120" s="2">
         <v>45017</v>
       </c>
-      <c r="B120" t="n">
+      <c r="B120">
         <v>-0.02562412309067441</v>
       </c>
-      <c r="C120" t="n">
+      <c r="C120">
         <v>0.005428539995270265</v>
       </c>
-      <c r="D120" t="n">
+      <c r="D120">
         <v>0.01706229436876328</v>
       </c>
-      <c r="E120" t="n">
+      <c r="E120">
         <v>0.003212794059900714</v>
       </c>
-      <c r="F120" t="n">
+      <c r="F120">
         <v>-0.001172996420938155</v>
       </c>
-      <c r="G120" t="n">
+      <c r="G120">
         <v>-0.03482741618281004</v>
       </c>
-      <c r="H120" t="inlineStr"/>
-      <c r="I120" t="n">
+      <c r="I120">
         <v>0.08429264072747755</v>
       </c>
-      <c r="J120" t="n">
+      <c r="J120">
         <v>-0.01454424802315268</v>
       </c>
     </row>
-    <row r="121">
-      <c r="A121" s="2" t="n">
+    <row r="121" spans="1:10">
+      <c r="A121" s="2">
         <v>45108</v>
       </c>
-      <c r="B121" t="n">
+      <c r="B121">
         <v>0.039367814571172</v>
       </c>
-      <c r="C121" t="n">
+      <c r="C121">
         <v>-0.01410183907392004</v>
       </c>
-      <c r="D121" t="n">
+      <c r="D121">
         <v>0.01300645644240661</v>
       </c>
-      <c r="E121" t="n">
+      <c r="E121">
         <v>0.003024588122264582</v>
       </c>
-      <c r="F121" t="n">
+      <c r="F121">
         <v>-0.03386375362837235</v>
       </c>
-      <c r="G121" t="n">
+      <c r="G121">
         <v>0.009360430285961341</v>
       </c>
-      <c r="H121" t="inlineStr"/>
-      <c r="I121" t="n">
+      <c r="I121">
         <v>0.01798306363105895</v>
       </c>
-      <c r="J121" t="n">
+      <c r="J121">
         <v>0.06295077116841785</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>